<commit_message>
bergupdate: changed a few things in CGHcall.R: it now uses X and Y chromosomes data, and handling plots is a bit easier now.
</commit_message>
<xml_diff>
--- a/docs/docs_I_received/par_laetitia/recap GIST projet GIRONDE - Copie ELIE.xlsx
+++ b/docs/docs_I_received/par_laetitia/recap GIST projet GIRONDE - Copie ELIE.xlsx
@@ -5,11 +5,11 @@
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="P:\Genetique\CGH array\Rendu CGH\2. GI GIST\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\e.bordron\Desktop\CGH-scoring\M2_internship_Bergonie\docs\docs_I_received\par_laetitia\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="120" windowWidth="28380" windowHeight="12150"/>
+    <workbookView xWindow="240" yWindow="120" windowWidth="28380" windowHeight="12150" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -301,11 +301,11 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <numFmts count="3">
-    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="164" formatCode="0.0"/>
-    <numFmt numFmtId="165" formatCode="0.00000000000000"/>
+    <numFmt numFmtId="164" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="0.0"/>
+    <numFmt numFmtId="166" formatCode="0.00000000000000"/>
   </numFmts>
   <fonts count="26" x14ac:knownFonts="1">
     <font>
@@ -4596,7 +4596,7 @@
     <xf numFmtId="0" fontId="1" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="43" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="164" fontId="23" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="8" borderId="8" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -5923,7 +5923,7 @@
     <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="38" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="38" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -5976,16 +5976,16 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="33" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="164" fontId="16" fillId="38" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="16" fillId="38" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="2" fontId="0" fillId="33" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="38" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="165" fontId="0" fillId="38" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="38" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -6006,7 +6006,7 @@
     <xf numFmtId="2" fontId="19" fillId="33" borderId="12" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="166" fontId="0" fillId="33" borderId="10" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="22" fillId="33" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -11265,8 +11265,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AA846"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -12843,7 +12843,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="N9" sqref="N9"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>

</xml_diff>